<commit_message>
Update data collection code and CMR14 data
</commit_message>
<xml_diff>
--- a/reference/CMR14/data_comparison_CMR14.xlsx
+++ b/reference/CMR14/data_comparison_CMR14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\reference\CMR14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7148928A-740D-4388-B261-85525B7A13C4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDC3B98-1621-475C-8316-66366D8E550B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="10" xr2:uid="{6F61AA73-B7AD-4D99-B7FC-61287560D07A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{6F61AA73-B7AD-4D99-B7FC-61287560D07A}"/>
   </bookViews>
   <sheets>
     <sheet name="papers_obs" sheetId="2" r:id="rId1"/>
@@ -32531,7 +32531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1189B2D8-8624-407F-9E92-FCEC195667E4}">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -39564,7 +39564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E19EFF1-F8A2-47AE-9878-83EFC0C12328}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -40141,7 +40141,7 @@
         <v>1.0080004295532643</v>
       </c>
       <c r="D59">
-        <f t="shared" ref="D3:D66" si="0">C59*$H$3+$I$3</f>
+        <f t="shared" ref="D59:D66" si="0">C59*$H$3+$I$3</f>
         <v>1.0005664850611231</v>
       </c>
     </row>

</xml_diff>